<commit_message>
added 6050 quasi cash
</commit_message>
<xml_diff>
--- a/inspired_mcc_codes.xlsx
+++ b/inspired_mcc_codes.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpicornell/devel/inspired/mcc-codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA24FB8-D5F1-6348-B2C7-C585EFA58264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C3B7D3-155C-754C-84BD-9D1EFF4B6A7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="660" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="540" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MCC" sheetId="2" r:id="rId1"/>
     <sheet name="Linked_fi_categories" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="prod_platform" localSheetId="0">MCC!$A$1:$C$985</definedName>
+    <definedName name="prod_platform" localSheetId="0">MCC!$A$1:$C$986</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4158" uniqueCount="2501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4161" uniqueCount="2503">
   <si>
     <t>category_id</t>
   </si>
@@ -7544,6 +7544,12 @@
   </si>
   <si>
     <t>Autograph Hotel</t>
+  </si>
+  <si>
+    <t>6050</t>
+  </si>
+  <si>
+    <t>Quasi Cash–Member Financial Institution</t>
   </si>
 </sst>
 </file>
@@ -8403,13 +8409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E985"/>
+  <dimension ref="A1:E986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B681" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B841" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="F866" sqref="F866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23983,64 +23989,67 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A866" s="1" t="s">
-        <v>1566</v>
+        <v>2501</v>
       </c>
       <c r="B866" s="4" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C866" s="4" t="s">
-        <v>1568</v>
+        <v>2502</v>
+      </c>
+      <c r="C866" t="s">
+        <v>2502</v>
       </c>
       <c r="D866">
-        <v>18020010</v>
+        <v>18020012</v>
       </c>
       <c r="E866" s="3" t="str">
         <f>VLOOKUP(D866,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Check Cashing</v>
+        <v>Service: Financial: Banking and Finance</v>
       </c>
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A867" s="1" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="B867" s="4" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="C867" s="4" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="D867">
-        <v>18020003</v>
+        <v>18020010</v>
       </c>
       <c r="E867" s="3" t="str">
         <f>VLOOKUP(D867,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Stock Brokers</v>
+        <v>Service: Financial: Check Cashing</v>
       </c>
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A868" s="1" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="B868" s="4" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C868" s="4" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="D868">
-        <v>18030000</v>
+        <v>18020003</v>
       </c>
       <c r="E868" s="3" t="str">
         <f>VLOOKUP(D868,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Insurance</v>
+        <v>Service: Financial: Stock Brokers</v>
       </c>
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A869" s="1" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="B869" s="4" t="s">
-        <v>1575</v>
+        <v>1572</v>
+      </c>
+      <c r="C869" s="4" t="s">
+        <v>1573</v>
       </c>
       <c r="D869">
         <v>18030000</v>
@@ -24052,13 +24061,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A870" s="1" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="B870" s="4" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C870" s="4" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="D870">
         <v>18030000</v>
@@ -24070,175 +24076,175 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A871" s="1" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="B871" s="4" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="C871" s="4" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="D871">
-        <v>18050003</v>
+        <v>18030000</v>
       </c>
       <c r="E871" s="3" t="str">
         <f>VLOOKUP(D871,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Real Estate: Real Estate Agents</v>
+        <v>Service: Insurance</v>
       </c>
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A872" s="1" t="s">
-        <v>2492</v>
+        <v>1579</v>
       </c>
       <c r="B872" s="4" t="s">
-        <v>2493</v>
+        <v>1580</v>
       </c>
       <c r="C872" s="4" t="s">
-        <v>2493</v>
+        <v>1580</v>
       </c>
       <c r="D872">
-        <v>21010000</v>
+        <v>18050003</v>
       </c>
       <c r="E872" s="3" t="str">
         <f>VLOOKUP(D872,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Transfer: Third Party</v>
+        <v>Service: Real Estate: Real Estate Agents</v>
       </c>
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A873" s="1" t="s">
-        <v>1886</v>
+        <v>2492</v>
       </c>
       <c r="B873" s="4" t="s">
-        <v>1887</v>
+        <v>2493</v>
       </c>
       <c r="C873" s="4" t="s">
-        <v>1888</v>
+        <v>2493</v>
       </c>
       <c r="D873">
-        <v>18020010</v>
+        <v>21010000</v>
       </c>
       <c r="E873" s="3" t="str">
         <f>VLOOKUP(D873,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Check Cashing</v>
+        <v>Transfer: Third Party</v>
       </c>
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A874" s="1" t="s">
-        <v>1892</v>
+        <v>1886</v>
       </c>
       <c r="B874" s="4" t="s">
-        <v>1893</v>
+        <v>1887</v>
       </c>
       <c r="C874" s="4" t="s">
-        <v>1893</v>
+        <v>1888</v>
       </c>
       <c r="D874">
-        <v>10000000</v>
+        <v>18020010</v>
       </c>
       <c r="E874" s="3" t="str">
         <f>VLOOKUP(D874,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Bank Fees</v>
+        <v>Service: Financial: Check Cashing</v>
       </c>
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A875" s="1" t="s">
-        <v>1581</v>
+        <v>1892</v>
       </c>
       <c r="B875" s="4" t="s">
-        <v>1582</v>
+        <v>1893</v>
       </c>
       <c r="C875" s="4" t="s">
-        <v>1583</v>
+        <v>1893</v>
       </c>
       <c r="D875">
-        <v>22012003</v>
+        <v>10000000</v>
       </c>
       <c r="E875" s="3" t="str">
         <f>VLOOKUP(D875,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Travel: Lodging: Hotels and Motels</v>
+        <v>Bank Fees</v>
       </c>
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A876" s="1" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="B876" s="4" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="C876" s="4" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D876">
-        <v>22012002</v>
+        <v>22012003</v>
       </c>
       <c r="E876" s="3" t="str">
         <f>VLOOKUP(D876,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Travel: Lodging: Lodges and Vacation Rentals</v>
+        <v>Travel: Lodging: Hotels and Motels</v>
       </c>
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A877" s="1" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B877" s="4" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C877" s="4" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="D877">
-        <v>17041000</v>
+        <v>22012002</v>
       </c>
       <c r="E877" s="3" t="str">
         <f>VLOOKUP(D877,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Sports and Recreation Camps</v>
+        <v>Travel: Lodging: Lodges and Vacation Rentals</v>
       </c>
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A878" s="1" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="B878" s="4" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="C878" s="4" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="D878">
-        <v>17007000</v>
+        <v>17041000</v>
       </c>
       <c r="E878" s="3" t="str">
         <f>VLOOKUP(D878,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Campgrounds and RV Parks</v>
+        <v>Recreation: Sports and Recreation Camps</v>
       </c>
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A879" s="1" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="B879" s="4" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="C879" s="4" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="D879">
-        <v>18045008</v>
+        <v>17007000</v>
       </c>
       <c r="E879" s="3" t="str">
         <f>VLOOKUP(D879,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Personal Care: Laundry and Garment Services</v>
+        <v>Recreation: Campgrounds and RV Parks</v>
       </c>
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A880" s="1" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="B880" s="4" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="C880" s="4" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="D880">
         <v>18045008</v>
@@ -24250,13 +24256,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A881" s="1" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="B881" s="4" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="C881" s="4" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="D881">
         <v>18045008</v>
@@ -24268,586 +24274,586 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A882" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="B882" s="4" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="C882" s="4" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="D882">
-        <v>18024025</v>
+        <v>18045008</v>
       </c>
       <c r="E882" s="3" t="str">
         <f>VLOOKUP(D882,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Home Improvement: Carpet and Flooring</v>
+        <v>Service: Personal Care: Laundry and Garment Services</v>
       </c>
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A883" s="1" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="B883" s="4" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="C883" s="4" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="D883">
-        <v>18047000</v>
+        <v>18024025</v>
       </c>
       <c r="E883" s="3" t="str">
         <f>VLOOKUP(D883,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Photography</v>
+        <v>Service: Home Improvement: Carpet and Flooring</v>
       </c>
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A884" s="1" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="B884" s="4" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="C884" s="4" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="D884">
-        <v>18045009</v>
+        <v>18047000</v>
       </c>
       <c r="E884" s="3" t="str">
         <f>VLOOKUP(D884,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Personal Care: Hair Salons and Barbers</v>
+        <v>Service: Photography</v>
       </c>
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A885" s="1" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="B885" s="4" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="C885" s="4" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
       <c r="D885">
-        <v>18011000</v>
+        <v>18045009</v>
       </c>
       <c r="E885" s="3" t="str">
         <f>VLOOKUP(D885,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Cleaning</v>
+        <v>Service: Personal Care: Hair Salons and Barbers</v>
       </c>
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A886" s="1" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
       <c r="B886" s="4" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="C886" s="4" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
       <c r="D886">
-        <v>18022000</v>
+        <v>18011000</v>
       </c>
       <c r="E886" s="3" t="str">
         <f>VLOOKUP(D886,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Funeral Services</v>
+        <v>Service: Cleaning</v>
       </c>
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A887" s="1" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="B887" s="4" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="C887" s="4" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="D887">
-        <v>18015000</v>
+        <v>18022000</v>
       </c>
       <c r="E887" s="3" t="str">
         <f>VLOOKUP(D887,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Dating and Escort</v>
+        <v>Service: Funeral Services</v>
       </c>
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A888" s="1" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
       <c r="B888" s="4" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="C888" s="4" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
       <c r="D888">
-        <v>18020001</v>
+        <v>18015000</v>
       </c>
       <c r="E888" s="3" t="str">
         <f>VLOOKUP(D888,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Taxes</v>
+        <v>Service: Dating and Escort</v>
       </c>
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A889" s="1" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="B889" s="4" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
       <c r="C889" s="4" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="D889">
-        <v>18014000</v>
+        <v>18020001</v>
       </c>
       <c r="E889" s="3" t="str">
         <f>VLOOKUP(D889,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Credit Counseling and Bankruptcy Services</v>
+        <v>Service: Financial: Taxes</v>
       </c>
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A890" s="1" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="B890" s="4" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
       <c r="C890" s="4" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="D890">
-        <v>19053000</v>
+        <v>18014000</v>
       </c>
       <c r="E890" s="3" t="str">
         <f>VLOOKUP(D890,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Wholesale</v>
+        <v>Service: Credit Counseling and Bankruptcy Services</v>
       </c>
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A891" s="1" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="B891" s="4" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="C891" s="4" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="D891">
-        <v>19016000</v>
+        <v>19053000</v>
       </c>
       <c r="E891" s="3" t="str">
         <f>VLOOKUP(D891,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Costumes</v>
+        <v>Shops: Wholesale</v>
       </c>
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A892" s="1" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="B892" s="4" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
       <c r="C892" s="4" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="D892">
-        <v>18045006</v>
+        <v>19016000</v>
       </c>
       <c r="E892" s="3" t="str">
         <f>VLOOKUP(D892,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Personal Care: Massage Clinics and Therapists</v>
+        <v>Shops: Costumes</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A893" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="B893" s="4" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="C893" s="4" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
       <c r="D893">
-        <v>18045003</v>
+        <v>18045006</v>
       </c>
       <c r="E893" s="3" t="str">
         <f>VLOOKUP(D893,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Personal Care: Spas</v>
+        <v>Service: Personal Care: Massage Clinics and Therapists</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A894" s="1" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="B894" s="4" t="s">
-        <v>2495</v>
+        <v>1631</v>
       </c>
       <c r="C894" s="4" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="D894">
-        <v>18045000</v>
+        <v>18045003</v>
       </c>
       <c r="E894" s="3" t="str">
         <f>VLOOKUP(D894,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Personal Care</v>
+        <v>Service: Personal Care: Spas</v>
       </c>
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A895" s="1" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="B895" s="4" t="s">
-        <v>1636</v>
+        <v>2495</v>
       </c>
       <c r="C895" s="4" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="D895">
-        <v>18001010</v>
+        <v>18045000</v>
       </c>
       <c r="E895" s="3" t="str">
         <f>VLOOKUP(D895,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Advertising and Marketing: Advertising Agencies and Media Buyers</v>
+        <v>Service: Personal Care</v>
       </c>
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A896" s="1" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="B896" s="4" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="C896" s="4" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="D896">
-        <v>18020008</v>
+        <v>18001010</v>
       </c>
       <c r="E896" s="3" t="str">
         <f>VLOOKUP(D896,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Credit Reporting</v>
+        <v>Service: Advertising and Marketing: Advertising Agencies and Media Buyers</v>
       </c>
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A897" s="1" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
       <c r="B897" s="4" t="s">
-        <v>1641</v>
+        <v>1638</v>
+      </c>
+      <c r="C897" s="4" t="s">
+        <v>1639</v>
       </c>
       <c r="D897">
-        <v>18008001</v>
+        <v>18020008</v>
       </c>
       <c r="E897" s="3" t="str">
         <f>VLOOKUP(D897,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Business Services: Printing and Publishing</v>
+        <v>Service: Financial: Credit Reporting</v>
       </c>
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A898" s="1" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="B898" s="4" t="s">
-        <v>1643</v>
-      </c>
-      <c r="C898" s="4" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="D898">
-        <v>18074000</v>
+        <v>18008001</v>
       </c>
       <c r="E898" s="3" t="str">
         <f>VLOOKUP(D898,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Art and Graphic Design</v>
+        <v>Service: Business Services: Printing and Publishing</v>
       </c>
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A899" s="1" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="B899" s="4" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="C899" s="4" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
       <c r="D899">
-        <v>18008001</v>
+        <v>18074000</v>
       </c>
       <c r="E899" s="3" t="str">
         <f>VLOOKUP(D899,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Business Services: Printing and Publishing</v>
+        <v>Service: Art and Graphic Design</v>
       </c>
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A900" s="1" t="s">
-        <v>1647</v>
+        <v>1644</v>
       </c>
       <c r="B900" s="4" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
       <c r="C900" s="4" t="s">
-        <v>1649</v>
+        <v>1646</v>
       </c>
       <c r="D900">
-        <v>18008000</v>
+        <v>18008001</v>
       </c>
       <c r="E900" s="3" t="str">
         <f>VLOOKUP(D900,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Business Services</v>
+        <v>Service: Business Services: Printing and Publishing</v>
       </c>
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A901" s="1" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
       <c r="B901" s="4" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="C901" s="4" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="D901">
-        <v>18024008</v>
+        <v>18008000</v>
       </c>
       <c r="E901" s="3" t="str">
         <f>VLOOKUP(D901,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Home Improvement: Pest Control</v>
+        <v>Service: Business Services</v>
       </c>
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A902" s="1" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="B902" s="4" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
       <c r="C902" s="4" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="D902">
-        <v>18011000</v>
+        <v>18024008</v>
       </c>
       <c r="E902" s="3" t="str">
         <f>VLOOKUP(D902,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Cleaning</v>
+        <v>Service: Home Improvement: Pest Control</v>
       </c>
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A903" s="1" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
       <c r="B903" s="4" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="C903" s="4" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
       <c r="D903">
-        <v>18016000</v>
+        <v>18011000</v>
       </c>
       <c r="E903" s="3" t="str">
         <f>VLOOKUP(D903,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Employment Agencies</v>
+        <v>Service: Cleaning</v>
       </c>
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A904" s="1" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
       <c r="B904" s="4" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="C904" s="4" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="D904">
-        <v>18059000</v>
+        <v>18016000</v>
       </c>
       <c r="E904" s="3" t="str">
         <f>VLOOKUP(D904,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Software Development</v>
+        <v>Service: Employment Agencies</v>
       </c>
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A905" s="1" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="B905" s="4" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="C905" s="4" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="D905">
-        <v>18012000</v>
+        <v>18059000</v>
       </c>
       <c r="E905" s="3" t="str">
         <f>VLOOKUP(D905,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Computers</v>
+        <v>Service: Software Development</v>
       </c>
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A906" s="1" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="B906" s="4" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="C906" s="4" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
       <c r="D906">
-        <v>18012001</v>
+        <v>18012000</v>
       </c>
       <c r="E906" s="3" t="str">
         <f>VLOOKUP(D906,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Computers: Maintenance and Repair</v>
+        <v>Service: Computers</v>
       </c>
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A907" s="1" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="B907" s="4" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="C907" s="4" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="D907">
-        <v>18001003</v>
+        <v>18012001</v>
       </c>
       <c r="E907" s="3" t="str">
         <f>VLOOKUP(D907,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Advertising and Marketing: Public Relations</v>
+        <v>Service: Computers: Maintenance and Repair</v>
       </c>
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A908" s="1" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="B908" s="4" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="C908" s="4" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
       <c r="D908">
-        <v>18057000</v>
+        <v>18001003</v>
       </c>
       <c r="E908" s="3" t="str">
         <f>VLOOKUP(D908,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Security and Safety</v>
+        <v>Service: Advertising and Marketing: Public Relations</v>
       </c>
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A909" s="1" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="B909" s="4" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="C909" s="4" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="D909">
-        <v>19022000</v>
+        <v>18057000</v>
       </c>
       <c r="E909" s="3" t="str">
         <f>VLOOKUP(D909,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Equipment Rental</v>
+        <v>Service: Security and Safety</v>
       </c>
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A910" s="1" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B910" s="4" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="C910" s="4" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="D910">
-        <v>18047000</v>
+        <v>19022000</v>
       </c>
       <c r="E910" s="3" t="str">
         <f>VLOOKUP(D910,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Photography</v>
+        <v>Shops: Equipment Rental</v>
       </c>
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A911" s="1" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="B911" s="4" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="C911" s="4" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="D911">
-        <v>18008000</v>
+        <v>18047000</v>
       </c>
       <c r="E911" s="3" t="str">
         <f>VLOOKUP(D911,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Business Services</v>
+        <v>Service: Photography</v>
       </c>
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A912" s="1" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="B912" s="4" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="C912" s="4" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="D912">
-        <v>22009000</v>
+        <v>18008000</v>
       </c>
       <c r="E912" s="3" t="str">
         <f>VLOOKUP(D912,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Travel: Gas Stations</v>
+        <v>Service: Business Services</v>
       </c>
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A913" s="1" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="B913" s="4" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="C913" s="4" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
       <c r="D913">
-        <v>22005000</v>
+        <v>22009000</v>
       </c>
       <c r="E913" s="3" t="str">
         <f>VLOOKUP(D913,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Travel: Car and Truck Rentals</v>
+        <v>Travel: Gas Stations</v>
       </c>
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A914" s="1" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="B914" s="4" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="C914" s="4" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="D914">
         <v>22005000</v>
@@ -24859,67 +24865,67 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A915" s="1" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
       <c r="B915" s="4" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="C915" s="4" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="D915">
-        <v>19005003</v>
+        <v>22005000</v>
       </c>
       <c r="E915" s="3" t="str">
         <f>VLOOKUP(D915,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Automotive: RVs and Motor Homes</v>
+        <v>Travel: Car and Truck Rentals</v>
       </c>
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A916" s="1" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="B916" s="4" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="C916" s="4" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="D916">
-        <v>22013000</v>
+        <v>19005003</v>
       </c>
       <c r="E916" s="3" t="str">
         <f>VLOOKUP(D916,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Travel: Parking</v>
+        <v>Shops: Automotive: RVs and Motor Homes</v>
       </c>
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A917" s="1" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B917" s="4" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="C917" s="4" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="D917">
-        <v>18006003</v>
+        <v>22013000</v>
       </c>
       <c r="E917" s="3" t="str">
         <f>VLOOKUP(D917,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Automotive: Maintenance and Repair</v>
+        <v>Travel: Parking</v>
       </c>
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A918" s="1" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="B918" s="4" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
       <c r="C918" s="4" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
       <c r="D918">
         <v>18006003</v>
@@ -24931,13 +24937,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A919" s="1" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
       <c r="B919" s="4" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="C919" s="4" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="D919">
         <v>18006003</v>
@@ -24949,13 +24955,13 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A920" s="1" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="B920" s="4" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="C920" s="4" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="D920">
         <v>18006003</v>
@@ -24967,85 +24973,85 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A921" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="B921" s="4" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="C921" s="4" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="D921">
-        <v>18006004</v>
+        <v>18006003</v>
       </c>
       <c r="E921" s="3" t="str">
         <f>VLOOKUP(D921,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Automotive: Car Wash and Detail</v>
+        <v>Service: Automotive: Maintenance and Repair</v>
       </c>
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A922" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="B922" s="4" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="C922" s="4" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="D922">
-        <v>18006001</v>
+        <v>18006004</v>
       </c>
       <c r="E922" s="3" t="str">
         <f>VLOOKUP(D922,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Automotive: Towing</v>
+        <v>Service: Automotive: Car Wash and Detail</v>
       </c>
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A923" s="1" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="B923" s="4" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="C923" s="4" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="D923">
-        <v>19013000</v>
+        <v>18006001</v>
       </c>
       <c r="E923" s="3" t="str">
         <f>VLOOKUP(D923,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Computers and Electronics</v>
+        <v>Service: Automotive: Towing</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A924" s="1" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="B924" s="4" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
       <c r="C924" s="4" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="D924">
-        <v>18053000</v>
+        <v>19013000</v>
       </c>
       <c r="E924" s="3" t="str">
         <f>VLOOKUP(D924,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Repair Services</v>
+        <v>Shops: Computers and Electronics</v>
       </c>
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A925" s="1" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="B925" s="4" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="C925" s="4" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="D925">
         <v>18053000</v>
@@ -25057,49 +25063,49 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A926" s="1" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="B926" s="4" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="C926" s="4" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="D926">
-        <v>19033000</v>
+        <v>18053000</v>
       </c>
       <c r="E926" s="3" t="str">
         <f>VLOOKUP(D926,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Jewelry and Watches</v>
+        <v>Service: Repair Services</v>
       </c>
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A927" s="1" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="B927" s="4" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="C927" s="4" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="D927">
-        <v>18053000</v>
+        <v>19033000</v>
       </c>
       <c r="E927" s="3" t="str">
         <f>VLOOKUP(D927,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Repair Services</v>
+        <v>Shops: Jewelry and Watches</v>
       </c>
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A928" s="1" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="B928" s="4" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="C928" s="4" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="D928">
         <v>18053000</v>
@@ -25111,13 +25117,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A929" s="1" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="B929" s="4" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="C929" s="4" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="D929">
         <v>18053000</v>
@@ -25129,460 +25135,463 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A930" s="1" t="s">
-        <v>1894</v>
+        <v>1729</v>
       </c>
       <c r="B930" s="4" t="s">
-        <v>1895</v>
+        <v>1730</v>
       </c>
       <c r="C930" s="4" t="s">
-        <v>1895</v>
+        <v>1731</v>
       </c>
       <c r="D930">
-        <v>17001014</v>
+        <v>18053000</v>
       </c>
       <c r="E930" s="3" t="str">
         <f>VLOOKUP(D930,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Casinos and Gaming</v>
+        <v>Service: Repair Services</v>
       </c>
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A931" s="1" t="s">
-        <v>1732</v>
+        <v>1894</v>
       </c>
       <c r="B931" s="4" t="s">
-        <v>1733</v>
+        <v>1895</v>
       </c>
       <c r="C931" s="4" t="s">
-        <v>1734</v>
+        <v>1895</v>
       </c>
       <c r="D931">
-        <v>18018001</v>
+        <v>17001014</v>
       </c>
       <c r="E931" s="3" t="str">
         <f>VLOOKUP(D931,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Entertainment: Media</v>
+        <v>Recreation: Arts and Entertainment: Casinos and Gaming</v>
       </c>
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A932" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B932" s="4" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="C932" s="4" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="D932">
-        <v>17001009</v>
+        <v>18018001</v>
       </c>
       <c r="E932" s="3" t="str">
         <f>VLOOKUP(D932,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Movie Theatres</v>
+        <v>Service: Entertainment: Media</v>
       </c>
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A933" s="1" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="B933" s="4" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="C933" s="4" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="D933">
-        <v>19036000</v>
+        <v>17001009</v>
       </c>
       <c r="E933" s="3" t="str">
         <f>VLOOKUP(D933,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Music, Video and DVD</v>
+        <v>Recreation: Arts and Entertainment: Movie Theatres</v>
       </c>
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A934" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="B934" s="4" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="C934" s="4" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="D934">
-        <v>17001012</v>
+        <v>19036000</v>
       </c>
       <c r="E934" s="3" t="str">
         <f>VLOOKUP(D934,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Dance Halls and Saloons</v>
+        <v>Shops: Music, Video and DVD</v>
       </c>
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A935" s="1" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="B935" s="4" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="C935" s="4" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="D935">
-        <v>17001000</v>
+        <v>17001012</v>
       </c>
       <c r="E935" s="3" t="str">
         <f>VLOOKUP(D935,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment</v>
+        <v>Recreation: Arts and Entertainment: Dance Halls and Saloons</v>
       </c>
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A936" s="1" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="B936" s="4" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
       <c r="C936" s="4" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="D936">
-        <v>17001002</v>
+        <v>17001000</v>
       </c>
       <c r="E936" s="3" t="str">
         <f>VLOOKUP(D936,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Symphony and Opera</v>
+        <v>Recreation: Arts and Entertainment</v>
       </c>
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A937" s="1" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="B937" s="4" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="C937" s="4" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="D937">
-        <v>17001016</v>
+        <v>17001002</v>
       </c>
       <c r="E937" s="3" t="str">
         <f>VLOOKUP(D937,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Billiards and Pool</v>
+        <v>Recreation: Arts and Entertainment: Symphony and Opera</v>
       </c>
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A938" s="1" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="B938" s="4" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="C938" s="4" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="D938">
-        <v>17001015</v>
+        <v>17001016</v>
       </c>
       <c r="E938" s="3" t="str">
         <f>VLOOKUP(D938,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Bowling</v>
+        <v>Recreation: Arts and Entertainment: Billiards and Pool</v>
       </c>
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A939" s="1" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="B939" s="4" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="C939" s="4" t="s">
-        <v>1755</v>
+        <v>1752</v>
       </c>
       <c r="D939">
-        <v>17042000</v>
+        <v>17001015</v>
       </c>
       <c r="E939" s="3" t="str">
         <f>VLOOKUP(D939,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Sports Clubs</v>
+        <v>Recreation: Arts and Entertainment: Bowling</v>
       </c>
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A940" s="1" t="s">
-        <v>1756</v>
+        <v>1753</v>
       </c>
       <c r="B940" s="4" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="C940" s="4" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="D940">
-        <v>17023001</v>
+        <v>17042000</v>
       </c>
       <c r="E940" s="3" t="str">
         <f>VLOOKUP(D940,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Landmarks: Monuments and Memorials</v>
+        <v>Recreation: Sports Clubs</v>
       </c>
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A941" s="1" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="B941" s="4" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="C941" s="4" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="D941">
-        <v>17015000</v>
+        <v>17023001</v>
       </c>
       <c r="E941" s="3" t="str">
         <f>VLOOKUP(D941,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Golf</v>
+        <v>Recreation: Landmarks: Monuments and Memorials</v>
       </c>
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A942" s="1" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="B942" s="4" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="C942" s="4" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="D942">
-        <v>19013001</v>
+        <v>17015000</v>
       </c>
       <c r="E942" s="3" t="str">
         <f>VLOOKUP(D942,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Computers and Electronics: Video Games</v>
+        <v>Recreation: Golf</v>
       </c>
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A943" s="1" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="B943" s="4" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="C943" s="4" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="D943">
-        <v>17001018</v>
+        <v>19013001</v>
       </c>
       <c r="E943" s="3" t="str">
         <f>VLOOKUP(D943,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Arcades and Amusement Parks</v>
+        <v>Shops: Computers and Electronics: Video Games</v>
       </c>
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A944" s="1" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="B944" s="4" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="C944" s="4" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="D944">
-        <v>17001014</v>
+        <v>17001018</v>
       </c>
       <c r="E944" s="3" t="str">
         <f>VLOOKUP(D944,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Casinos and Gaming</v>
+        <v>Recreation: Arts and Entertainment: Arcades and Amusement Parks</v>
       </c>
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A945" s="1" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="B945" s="4" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="C945" s="4" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="D945">
-        <v>17001018</v>
+        <v>17001014</v>
       </c>
       <c r="E945" s="3" t="str">
         <f>VLOOKUP(D945,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Arcades and Amusement Parks</v>
+        <v>Recreation: Arts and Entertainment: Casinos and Gaming</v>
       </c>
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A946" s="1" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B946" s="4" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C946" s="4" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="D946">
-        <v>17042000</v>
+        <v>17001018</v>
       </c>
       <c r="E946" s="3" t="str">
         <f>VLOOKUP(D946,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Sports Clubs</v>
+        <v>Recreation: Arts and Entertainment: Arcades and Amusement Parks</v>
       </c>
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A947" s="1" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="B947" s="4" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="C947" s="4" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="D947">
-        <v>17001019</v>
+        <v>17042000</v>
       </c>
       <c r="E947" s="3" t="str">
         <f>VLOOKUP(D947,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Arts and Entertainment: Aquarium</v>
+        <v>Recreation: Sports Clubs</v>
       </c>
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A948" s="1" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="B948" s="4" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="C948" s="4" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="D948">
-        <v>17042000</v>
+        <v>17001019</v>
       </c>
       <c r="E948" s="3" t="str">
         <f>VLOOKUP(D948,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Recreation: Sports Clubs</v>
+        <v>Recreation: Arts and Entertainment: Aquarium</v>
       </c>
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A949" s="1" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="B949" s="4" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="C949" s="4" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
       <c r="D949">
-        <v>14002000</v>
+        <v>17042000</v>
       </c>
       <c r="E949" s="3" t="str">
         <f>VLOOKUP(D949,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Physicians</v>
+        <v>Recreation: Sports Clubs</v>
       </c>
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A950" s="1" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="B950" s="4" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="C950" s="4" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="D950">
-        <v>14001012</v>
+        <v>14002000</v>
       </c>
       <c r="E950" s="3" t="str">
         <f>VLOOKUP(D950,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Dentists</v>
+        <v>Healthcare: Physicians</v>
       </c>
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A951" s="1" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="B951" s="4" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="C951" s="4" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="D951">
-        <v>14001016</v>
+        <v>14001012</v>
       </c>
       <c r="E951" s="3" t="str">
         <f>VLOOKUP(D951,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Alternative Medicine</v>
+        <v>Healthcare: Healthcare Services: Dentists</v>
       </c>
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A952" s="1" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="B952" s="4" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="C952" s="4" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="D952">
-        <v>14001014</v>
+        <v>14001016</v>
       </c>
       <c r="E952" s="3" t="str">
         <f>VLOOKUP(D952,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Chiropractors</v>
+        <v>Healthcare: Healthcare Services: Alternative Medicine</v>
       </c>
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A953" s="1" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="B953" s="4" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="C953" s="4" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="D953">
-        <v>14001005</v>
+        <v>14001014</v>
       </c>
       <c r="E953" s="3" t="str">
         <f>VLOOKUP(D953,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Optometrists</v>
+        <v>Healthcare: Healthcare Services: Chiropractors</v>
       </c>
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A954" s="1" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="B954" s="4" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C954" s="4" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="D954">
-        <v>19029000</v>
+        <v>14001005</v>
       </c>
       <c r="E954" s="3" t="str">
         <f>VLOOKUP(D954,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Shops: Glasses and Optometrist</v>
+        <v>Healthcare: Healthcare Services: Optometrists</v>
       </c>
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A955" s="1" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="B955" s="4" t="s">
-        <v>2496</v>
+        <v>1794</v>
+      </c>
+      <c r="C955" s="4" t="s">
+        <v>1795</v>
       </c>
       <c r="D955">
         <v>19029000</v>
@@ -25594,139 +25603,136 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A956" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B956" s="4" t="s">
-        <v>1798</v>
-      </c>
-      <c r="C956" s="4" t="s">
-        <v>1799</v>
+        <v>2496</v>
       </c>
       <c r="D956">
-        <v>14001003</v>
+        <v>19029000</v>
       </c>
       <c r="E956" s="3" t="str">
         <f>VLOOKUP(D956,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Podiatrists</v>
+        <v>Shops: Glasses and Optometrist</v>
       </c>
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A957" s="1" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="B957" s="4" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="C957" s="4" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="D957">
-        <v>14001007</v>
+        <v>14001003</v>
       </c>
       <c r="E957" s="3" t="str">
         <f>VLOOKUP(D957,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Nurses</v>
+        <v>Healthcare: Healthcare Services: Podiatrists</v>
       </c>
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A958" s="1" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="B958" s="4" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="C958" s="4" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
       <c r="D958">
-        <v>14001010</v>
+        <v>14001007</v>
       </c>
       <c r="E958" s="3" t="str">
         <f>VLOOKUP(D958,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Hospitals, Clinics and Medical Centers</v>
+        <v>Healthcare: Healthcare Services: Nurses</v>
       </c>
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A959" s="1" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="B959" s="4" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="C959" s="4" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="D959">
-        <v>14001009</v>
+        <v>14001010</v>
       </c>
       <c r="E959" s="3" t="str">
         <f>VLOOKUP(D959,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services: Medical Supplies and Labs</v>
+        <v>Healthcare: Healthcare Services: Hospitals, Clinics and Medical Centers</v>
       </c>
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A960" s="1" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="B960" s="4" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="C960" s="4" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="D960">
-        <v>14001000</v>
+        <v>14001009</v>
       </c>
       <c r="E960" s="3" t="str">
         <f>VLOOKUP(D960,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Healthcare: Healthcare Services</v>
+        <v>Healthcare: Healthcare Services: Medical Supplies and Labs</v>
       </c>
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A961" s="1" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="B961" s="4" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="C961" s="4" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="D961">
-        <v>18033000</v>
+        <v>14001000</v>
       </c>
       <c r="E961" s="3" t="str">
         <f>VLOOKUP(D961,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Legal</v>
+        <v>Healthcare: Healthcare Services</v>
       </c>
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A962" s="1" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="B962" s="4" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="C962" s="4" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="D962">
-        <v>12008003</v>
+        <v>18033000</v>
       </c>
       <c r="E962" s="3" t="str">
         <f>VLOOKUP(D962,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Education: Primary and Secondary Schools</v>
+        <v>Service: Legal</v>
       </c>
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A963" s="1" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="B963" s="4" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="C963" s="4" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="D963">
         <v>12008003</v>
@@ -25738,13 +25744,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A964" s="1" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
       <c r="B964" s="4" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="C964" s="4" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="D964">
         <v>12008003</v>
@@ -25756,13 +25762,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A965" s="1" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="B965" s="4" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="C965" s="4" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
       <c r="D965">
         <v>12008003</v>
@@ -25774,103 +25780,103 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A966" s="1" t="s">
-        <v>1825</v>
+        <v>1822</v>
       </c>
       <c r="B966" s="4" t="s">
-        <v>1826</v>
+        <v>1823</v>
       </c>
       <c r="C966" s="4" t="s">
-        <v>1827</v>
+        <v>1824</v>
       </c>
       <c r="D966">
-        <v>12008001</v>
+        <v>12008003</v>
       </c>
       <c r="E966" s="3" t="str">
         <f>VLOOKUP(D966,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Education: Vocational Schools</v>
+        <v>Community: Education: Primary and Secondary Schools</v>
       </c>
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A967" s="1" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
       <c r="B967" s="4" t="s">
-        <v>1829</v>
+        <v>1826</v>
       </c>
       <c r="C967" s="4" t="s">
-        <v>1830</v>
+        <v>1827</v>
       </c>
       <c r="D967">
-        <v>12008000</v>
+        <v>12008001</v>
       </c>
       <c r="E967" s="3" t="str">
         <f>VLOOKUP(D967,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Education</v>
+        <v>Community: Education: Vocational Schools</v>
       </c>
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A968" s="1" t="s">
-        <v>1831</v>
+        <v>1828</v>
       </c>
       <c r="B968" s="4" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="C968" s="4" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="D968">
-        <v>12005000</v>
+        <v>12008000</v>
       </c>
       <c r="E968" s="3" t="str">
         <f>VLOOKUP(D968,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Day Care and Preschools</v>
+        <v>Community: Education</v>
       </c>
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A969" s="1" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="B969" s="4" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
       <c r="C969" s="4" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="D969">
-        <v>12015003</v>
+        <v>12005000</v>
       </c>
       <c r="E969" s="3" t="str">
         <f>VLOOKUP(D969,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Organizations and Associations: Charities and Non-Profits</v>
+        <v>Community: Day Care and Preschools</v>
       </c>
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A970" s="1" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
       <c r="B970" s="4" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="C970" s="4" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="D970">
-        <v>12015000</v>
+        <v>12015003</v>
       </c>
       <c r="E970" s="3" t="str">
         <f>VLOOKUP(D970,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Organizations and Associations</v>
+        <v>Community: Organizations and Associations: Charities and Non-Profits</v>
       </c>
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A971" s="1" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="B971" s="4" t="s">
-        <v>1840</v>
+        <v>1837</v>
       </c>
       <c r="C971" s="4" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="D971">
         <v>12015000</v>
@@ -25882,49 +25888,49 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A972" s="1" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="B972" s="4" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="C972" s="4" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="D972">
-        <v>12018000</v>
+        <v>12015000</v>
       </c>
       <c r="E972" s="3" t="str">
         <f>VLOOKUP(D972,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Religious</v>
+        <v>Community: Organizations and Associations</v>
       </c>
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A973" s="1" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="B973" s="4" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="C973" s="4" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="D973">
-        <v>12015000</v>
+        <v>12018000</v>
       </c>
       <c r="E973" s="3" t="str">
         <f>VLOOKUP(D973,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Organizations and Associations</v>
+        <v>Community: Religious</v>
       </c>
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A974" s="1" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="B974" s="4" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="C974" s="4" t="s">
-        <v>1847</v>
+        <v>1844</v>
       </c>
       <c r="D974">
         <v>12015000</v>
@@ -25936,205 +25942,223 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A975" s="1" t="s">
-        <v>1848</v>
+        <v>1845</v>
       </c>
       <c r="B975" s="4" t="s">
-        <v>1849</v>
+        <v>1846</v>
       </c>
       <c r="C975" s="4" t="s">
-        <v>1850</v>
+        <v>1847</v>
       </c>
       <c r="D975">
-        <v>18054000</v>
+        <v>12015000</v>
       </c>
       <c r="E975" s="3" t="str">
         <f>VLOOKUP(D975,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Research</v>
+        <v>Community: Organizations and Associations</v>
       </c>
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A976" s="1" t="s">
-        <v>1851</v>
+        <v>1848</v>
       </c>
       <c r="B976" s="4" t="s">
-        <v>1852</v>
+        <v>1849</v>
       </c>
       <c r="C976" s="4" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="D976">
-        <v>18050007</v>
+        <v>18054000</v>
       </c>
       <c r="E976" s="3" t="str">
         <f>VLOOKUP(D976,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Real Estate: Building and Land Surveyors</v>
+        <v>Service: Research</v>
       </c>
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A977" s="1" t="s">
-        <v>1854</v>
+        <v>1851</v>
       </c>
       <c r="B977" s="4" t="s">
-        <v>1855</v>
+        <v>1852</v>
       </c>
       <c r="C977" s="4" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
       <c r="D977">
-        <v>18020014</v>
+        <v>18050007</v>
       </c>
       <c r="E977" s="3" t="str">
         <f>VLOOKUP(D977,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service: Financial: Accounting and Bookkeeping</v>
+        <v>Service: Real Estate: Building and Land Surveyors</v>
       </c>
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A978" s="1" t="s">
-        <v>1857</v>
+        <v>1854</v>
       </c>
       <c r="B978" s="4" t="s">
-        <v>1858</v>
+        <v>1855</v>
       </c>
       <c r="C978" s="4" t="s">
-        <v>1859</v>
+        <v>1856</v>
       </c>
       <c r="D978">
-        <v>18000000</v>
+        <v>18020014</v>
       </c>
       <c r="E978" s="3" t="str">
         <f>VLOOKUP(D978,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Service</v>
+        <v>Service: Financial: Accounting and Bookkeeping</v>
       </c>
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A979" s="1" t="s">
-        <v>1860</v>
+        <v>1857</v>
       </c>
       <c r="B979" s="4" t="s">
-        <v>1861</v>
+        <v>1858</v>
       </c>
       <c r="C979" s="4" t="s">
-        <v>1862</v>
+        <v>1859</v>
       </c>
       <c r="D979">
-        <v>12004000</v>
+        <v>18000000</v>
       </c>
       <c r="E979" s="3" t="str">
         <f>VLOOKUP(D979,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Courts</v>
+        <v>Service</v>
       </c>
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A980" s="1" t="s">
-        <v>1863</v>
+        <v>1860</v>
       </c>
       <c r="B980" s="4" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="C980" s="4" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="D980">
-        <v>12009000</v>
+        <v>12004000</v>
       </c>
       <c r="E980" s="3" t="str">
         <f>VLOOKUP(D980,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Government Departments and Agencies</v>
+        <v>Community: Courts</v>
       </c>
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A981" s="1" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="B981" s="4" t="s">
-        <v>1867</v>
+        <v>1864</v>
       </c>
       <c r="C981" s="4" t="s">
-        <v>1868</v>
+        <v>1865</v>
       </c>
       <c r="D981">
-        <v>12004000</v>
+        <v>12009000</v>
       </c>
       <c r="E981" s="3" t="str">
         <f>VLOOKUP(D981,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Courts</v>
+        <v>Community: Government Departments and Agencies</v>
       </c>
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A982" s="1" t="s">
-        <v>1869</v>
+        <v>1866</v>
       </c>
       <c r="B982" s="4" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
       <c r="C982" s="4" t="s">
-        <v>1871</v>
+        <v>1868</v>
       </c>
       <c r="D982">
-        <v>20000000</v>
+        <v>12004000</v>
       </c>
       <c r="E982" s="3" t="str">
         <f>VLOOKUP(D982,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Tax</v>
+        <v>Community: Courts</v>
       </c>
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A983" s="1" t="s">
-        <v>1872</v>
+        <v>1869</v>
       </c>
       <c r="B983" s="4" t="s">
-        <v>1873</v>
+        <v>1870</v>
       </c>
       <c r="C983" s="4" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
       <c r="D983">
-        <v>12009000</v>
+        <v>20000000</v>
       </c>
       <c r="E983" s="3" t="str">
         <f>VLOOKUP(D983,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Government Departments and Agencies</v>
+        <v>Tax</v>
       </c>
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A984" s="1" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
       <c r="B984" s="4" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="C984" s="4" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="D984">
-        <v>12016000</v>
+        <v>12009000</v>
       </c>
       <c r="E984" s="3" t="str">
         <f>VLOOKUP(D984,Linked_fi_categories!$A:$C,3,TRUE)</f>
-        <v>Community: Post Offices</v>
+        <v>Community: Government Departments and Agencies</v>
       </c>
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A985" s="1" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B985" s="4" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="C985" s="4" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="D985">
-        <v>12009000</v>
+        <v>12016000</v>
       </c>
       <c r="E985" s="3" t="str">
         <f>VLOOKUP(D985,Linked_fi_categories!$A:$C,3,TRUE)</f>
+        <v>Community: Post Offices</v>
+      </c>
+    </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A986" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B986" s="4" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C986" s="4" t="s">
+        <v>1879</v>
+      </c>
+      <c r="D986">
+        <v>12009000</v>
+      </c>
+      <c r="E986" s="3" t="str">
+        <f>VLOOKUP(D986,Linked_fi_categories!$A:$C,3,TRUE)</f>
         <v>Community: Government Departments and Agencies</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E985">
-    <sortCondition ref="A2:A985"/>
+  <sortState ref="A2:E986">
+    <sortCondition ref="A2:A986"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -26145,8 +26169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C603"/>
   <sheetViews>
-    <sheetView topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="A561" sqref="A561"/>
+    <sheetView topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="C320" sqref="C320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>